<commit_message>
Update edited session - 2025-12-07T10:16:56.307Z - Cache Bust ID: 1765102616307lnys60bbo
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Dermatology_scanner1765056425812_795f4daa84a2f6b8fd4fd7e7d3270b4b8fdb612e669472888fc82a779fddb58d.xlsx
+++ b/log_history/Y4_B2526_Dermatology_scanner1765056425812_795f4daa84a2f6b8fd4fd7e7d3270b4b8fdb612e669472888fc82a779fddb58d.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1122,489 +1122,9 @@
         <v>nadahassanein99@hotmail.com</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="str">
-        <v>200897</v>
-      </c>
-      <c r="B37" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C37" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D37" t="str">
-        <v>12:10:49</v>
-      </c>
-      <c r="E37" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F37" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>201390</v>
-      </c>
-      <c r="B38" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C38" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D38" t="str">
-        <v>12:11:19</v>
-      </c>
-      <c r="E38" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F38" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>201563</v>
-      </c>
-      <c r="B39" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C39" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D39" t="str">
-        <v>12:12:00</v>
-      </c>
-      <c r="E39" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F39" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="str">
-        <v>200866</v>
-      </c>
-      <c r="B40" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C40" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D40" t="str">
-        <v>12:12:07</v>
-      </c>
-      <c r="E40" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F40" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="str">
-        <v>200997</v>
-      </c>
-      <c r="B41" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C41" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D41" t="str">
-        <v>12:12:17</v>
-      </c>
-      <c r="E41" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F41" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="str">
-        <v>201026</v>
-      </c>
-      <c r="B42" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C42" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D42" t="str">
-        <v>12:12:21</v>
-      </c>
-      <c r="E42" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F42" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="str">
-        <v>200762</v>
-      </c>
-      <c r="B43" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C43" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D43" t="str">
-        <v>12:12:43</v>
-      </c>
-      <c r="E43" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F43" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="str">
-        <v>200727</v>
-      </c>
-      <c r="B44" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C44" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D44" t="str">
-        <v>12:12:53</v>
-      </c>
-      <c r="E44" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F44" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="str">
-        <v>200708</v>
-      </c>
-      <c r="B45" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C45" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D45" t="str">
-        <v>12:13:00</v>
-      </c>
-      <c r="E45" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F45" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="str">
-        <v>201065</v>
-      </c>
-      <c r="B46" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C46" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D46" t="str">
-        <v>12:13:08</v>
-      </c>
-      <c r="E46" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F46" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="str">
-        <v>201328</v>
-      </c>
-      <c r="B47" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C47" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D47" t="str">
-        <v>12:13:12</v>
-      </c>
-      <c r="E47" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F47" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="str">
-        <v>200905</v>
-      </c>
-      <c r="B48" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C48" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D48" t="str">
-        <v>12:13:16</v>
-      </c>
-      <c r="E48" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F48" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="str">
-        <v>200869</v>
-      </c>
-      <c r="B49" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C49" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D49" t="str">
-        <v>12:13:26</v>
-      </c>
-      <c r="E49" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F49" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="str">
-        <v>200943</v>
-      </c>
-      <c r="B50" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C50" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D50" t="str">
-        <v>12:13:32</v>
-      </c>
-      <c r="E50" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F50" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="str">
-        <v>200852</v>
-      </c>
-      <c r="B51" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C51" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D51" t="str">
-        <v>12:13:36</v>
-      </c>
-      <c r="E51" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F51" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="str">
-        <v>201495</v>
-      </c>
-      <c r="B52" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C52" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D52" t="str">
-        <v>12:13:49</v>
-      </c>
-      <c r="E52" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F52" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="str">
-        <v>201190</v>
-      </c>
-      <c r="B53" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C53" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D53" t="str">
-        <v>12:13:59</v>
-      </c>
-      <c r="E53" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F53" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="str">
-        <v>201197</v>
-      </c>
-      <c r="B54" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C54" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D54" t="str">
-        <v>12:14:42</v>
-      </c>
-      <c r="E54" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F54" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="str">
-        <v>201255</v>
-      </c>
-      <c r="B55" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C55" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D55" t="str">
-        <v>12:14:50</v>
-      </c>
-      <c r="E55" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F55" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="str">
-        <v>200438</v>
-      </c>
-      <c r="B56" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C56" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D56" t="str">
-        <v>12:15:06</v>
-      </c>
-      <c r="E56" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F56" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="str">
-        <v>200858</v>
-      </c>
-      <c r="B57" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C57" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D57" t="str">
-        <v>12:15:11</v>
-      </c>
-      <c r="E57" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F57" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="str">
-        <v>200458</v>
-      </c>
-      <c r="B58" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C58" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D58" t="str">
-        <v>12:15:15</v>
-      </c>
-      <c r="E58" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F58" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="str">
-        <v>200914</v>
-      </c>
-      <c r="B59" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C59" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D59" t="str">
-        <v>12:15:18</v>
-      </c>
-      <c r="E59" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F59" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="str">
-        <v>201513</v>
-      </c>
-      <c r="B60" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C60" t="str">
-        <v>07/12/2025</v>
-      </c>
-      <c r="D60" t="str">
-        <v>12:15:38</v>
-      </c>
-      <c r="E60" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F60" t="str">
-        <v>nadahassanein99@hotmail.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F60"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F36"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>